<commit_message>
Close to ready, many changes
</commit_message>
<xml_diff>
--- a/Outline and To Do.xlsx
+++ b/Outline and To Do.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justj\JUCE\MYCODE\Audio-programming-with-VST-and-JUCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B133FDB-7852-4EB0-8889-8CB61188F769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2361E8DF-B14D-4021-83BF-93D9F13F277A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="21786" windowHeight="13866" xr2:uid="{F4FE9173-A103-4191-B358-E75A6D4277C5}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="21786" windowHeight="13866" activeTab="1" xr2:uid="{F4FE9173-A103-4191-B358-E75A6D4277C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Lectures" sheetId="1" r:id="rId1"/>
-    <sheet name="Assignments" sheetId="2" r:id="rId2"/>
-    <sheet name="To Do" sheetId="3" r:id="rId3"/>
-    <sheet name="Code" sheetId="5" r:id="rId4"/>
-    <sheet name="waa reduced" sheetId="7" r:id="rId5"/>
-    <sheet name="Web Audio" sheetId="6" r:id="rId6"/>
-    <sheet name="Phase vocoder" sheetId="8" r:id="rId7"/>
+    <sheet name="To Do" sheetId="3" r:id="rId2"/>
+    <sheet name="Code" sheetId="5" r:id="rId3"/>
+    <sheet name="waa reduced" sheetId="7" r:id="rId4"/>
+    <sheet name="Web Audio" sheetId="6" r:id="rId5"/>
+    <sheet name="Phase vocoder" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,60 +41,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="303">
-  <si>
-    <t>DAFX</t>
-  </si>
-  <si>
-    <t>ANDREW</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="287">
   <si>
     <t>Hello World</t>
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>ntroduction to Web Audio API</t>
-  </si>
-  <si>
-    <t>Recording a Beep</t>
-  </si>
-  <si>
-    <t>Audio effect analysis</t>
-  </si>
-  <si>
-    <t>Multiband dynamic range compression</t>
-  </si>
-  <si>
-    <t>Graphic EQ</t>
-  </si>
-  <si>
-    <t>Pluckable string / Karplus Strong</t>
-  </si>
-  <si>
-    <t>Working with worklets</t>
-  </si>
-  <si>
-    <t>Will</t>
-  </si>
-  <si>
-    <t>Stick slip friction</t>
-  </si>
-  <si>
-    <t>Original audio programming</t>
-  </si>
-  <si>
-    <t>sound design</t>
-  </si>
-  <si>
-    <t>Synth filter</t>
-  </si>
-  <si>
-    <t>Drum machine</t>
-  </si>
-  <si>
-    <t>Revised</t>
   </si>
   <si>
     <t>Topic</t>
@@ -1045,9 +996,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1085,7 +1036,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1191,7 +1142,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1333,7 +1284,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1343,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E90A2B3-29B0-4989-8060-67E082361C06}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1359,22 +1310,22 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.5">
@@ -1382,19 +1333,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2">
         <v>13</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.5">
@@ -1402,13 +1353,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2">
         <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -1417,13 +1368,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
         <v>11</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.5">
@@ -1431,13 +1382,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2">
         <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.5">
@@ -1445,13 +1396,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F6" s="2">
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H6" s="2">
         <f>SUM(F2:F6)</f>
@@ -1463,10 +1414,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.5">
@@ -1474,19 +1425,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F8" s="2">
         <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.5">
@@ -1494,13 +1445,13 @@
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F9" s="2">
         <v>8</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.5">
@@ -1508,13 +1459,13 @@
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2">
         <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.5">
@@ -1522,13 +1473,13 @@
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2">
         <v>7</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11" s="2">
         <f>SUM(F8:F11)</f>
@@ -1540,19 +1491,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="F12" s="2">
         <v>29</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.5">
@@ -1560,13 +1511,13 @@
         <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F13" s="2">
         <v>6</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J13" s="4"/>
     </row>
@@ -1575,13 +1526,13 @@
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F14" s="2">
         <v>10</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.5">
@@ -1589,13 +1540,13 @@
         <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F15" s="2">
         <v>19</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.5">
@@ -1603,7 +1554,10 @@
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="F16" s="2">
+        <v>29</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -1612,22 +1566,22 @@
         <v>7</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2">
         <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.5">
@@ -1635,10 +1589,10 @@
         <v>8</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.5">
@@ -1646,10 +1600,13 @@
         <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
+      </c>
+      <c r="F20" s="2">
+        <v>11</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.5">
@@ -1657,10 +1614,10 @@
         <v>10</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.5">
@@ -1668,7 +1625,10 @@
         <v>11</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>42</v>
+        <v>26</v>
+      </c>
+      <c r="F22" s="2">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.5">
@@ -1676,35 +1636,35 @@
         <v>12</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2">
         <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="F24" s="2">
         <v>23</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B25" s="2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C25" s="2">
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.5">
@@ -1712,7 +1672,7 @@
         <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.5">
@@ -1720,7 +1680,7 @@
         <v>15</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.5">
@@ -1728,13 +1688,13 @@
         <v>16</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F28" s="2">
         <v>33</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.5">
@@ -1742,7 +1702,7 @@
         <v>18</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F29" s="2">
         <v>36</v>
@@ -1750,13 +1710,13 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B30" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C30" s="2">
         <v>19</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F30" s="2">
         <v>15</v>
@@ -1767,7 +1727,7 @@
         <v>19</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="F31" s="2">
         <v>23</v>
@@ -1778,7 +1738,7 @@
         <v>19</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F32" s="2">
         <v>21</v>
@@ -1794,7 +1754,7 @@
         <v>20</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.5">
@@ -1802,32 +1762,32 @@
         <v>17</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="F36" s="2">
         <f>SUM(F1:F35)</f>
-        <v>311</v>
+        <v>362</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.5">
       <c r="C37" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.5">
       <c r="C38" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1836,169 +1796,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD531BE-CC01-41A0-A1B1-002E4E8CA59F}">
-  <dimension ref="A1:E19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="32.5859375" customWidth="1"/>
-    <col min="2" max="5" width="11.64453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DE14E8-2123-479D-80B5-4514ECC0BBC7}">
   <dimension ref="B2:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2006,22 +1807,22 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B2" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B3" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2029,7 +1830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDF5EB3-DB43-4FA4-9E26-95B4D5E8C0C0}">
   <dimension ref="A1:M55"/>
   <sheetViews>
@@ -2049,45 +1850,45 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B2" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D2" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
@@ -2097,10 +1898,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B3" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="G3" s="5">
         <v>1</v>
@@ -2110,10 +1911,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D4" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="I4" s="5">
         <v>1</v>
@@ -2123,10 +1924,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D5" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="F5" s="5">
         <v>1</v>
@@ -2136,10 +1937,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B6" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D6" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="F6" s="5">
         <v>1</v>
@@ -2149,10 +1950,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B7" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D7" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="F7" s="5">
         <v>1</v>
@@ -2162,10 +1963,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D8" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="F8" s="5">
         <v>1</v>
@@ -2175,10 +1976,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B9" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="F9" s="5">
         <v>1</v>
@@ -2188,10 +1989,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B10" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D10" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="F10" s="5">
         <v>1</v>
@@ -2201,10 +2002,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D11" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="F11" s="5">
         <v>1</v>
@@ -2214,10 +2015,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D12" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -2230,13 +2031,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="F13" s="5">
         <v>1</v>
@@ -2247,16 +2048,16 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="F14" s="5">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.5">
@@ -2264,16 +2065,16 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="F15" s="5">
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.5">
@@ -2281,13 +2082,13 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F16" s="5">
         <v>1</v>
@@ -2298,13 +2099,13 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="I17" s="5">
         <v>1</v>
@@ -2315,13 +2116,13 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F18" s="5">
         <v>1</v>
@@ -2344,13 +2145,13 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="F19" s="5">
         <v>1</v>
@@ -2373,13 +2174,13 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F20" s="5">
         <v>1</v>
@@ -2402,13 +2203,13 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="F21" s="5">
         <v>1</v>
@@ -2431,13 +2232,13 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F22" s="5">
         <v>1</v>
@@ -2460,13 +2261,13 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="F23" s="5">
         <v>1</v>
@@ -2489,13 +2290,13 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F24" s="5">
         <v>1</v>
@@ -2518,13 +2319,13 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F25" s="5">
         <v>1</v>
@@ -2547,13 +2348,13 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="G26" s="5">
         <v>1</v>
@@ -2570,13 +2371,13 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="F27" s="5">
         <v>1</v>
@@ -2599,13 +2400,13 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="F28" s="5">
         <v>1</v>
@@ -2628,19 +2429,19 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="F29" s="5">
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.5">
@@ -2648,13 +2449,13 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="F30" s="5">
         <v>1</v>
@@ -2668,13 +2469,13 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D31" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="F31" s="5">
         <v>1</v>
@@ -2694,13 +2495,13 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="F32" s="5">
         <v>1</v>
@@ -2711,13 +2512,13 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F33" s="5">
         <v>1</v>
@@ -2740,16 +2541,16 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="E34" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="F34" s="5">
         <v>1</v>
@@ -2763,16 +2564,16 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D35" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="E35" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="F35" s="5">
         <v>1</v>
@@ -2792,16 +2593,16 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E36" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="F36" s="5">
         <v>1</v>
@@ -2815,16 +2616,16 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E37" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="F37" s="5">
         <v>1</v>
@@ -2838,13 +2639,13 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D38" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="G38" s="5">
         <v>1</v>
@@ -2858,13 +2659,13 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G39" s="5">
         <v>1</v>
@@ -2878,13 +2679,13 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D40" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="F40" s="5">
         <v>1</v>
@@ -2895,13 +2696,13 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F41" s="5">
         <v>1</v>
@@ -2915,13 +2716,13 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="F42" s="5">
         <v>1</v>
@@ -2935,13 +2736,13 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D43" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="I43" s="5">
         <v>1</v>
@@ -2952,13 +2753,13 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D44" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="G44" s="5">
         <v>1</v>
@@ -2967,12 +2768,12 @@
         <v>1</v>
       </c>
       <c r="L44" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="F46" s="7">
         <f>SUM(F2:F45)</f>
@@ -2997,47 +2798,47 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.5">
       <c r="B47" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.5">
       <c r="B48" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B49" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B50" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B51" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B52" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B53" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B54" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B55" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3046,7 +2847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B61ACB0-25EE-4420-AB81-7367422D4FA5}">
   <dimension ref="B1:C236"/>
   <sheetViews>
@@ -3062,482 +2863,482 @@
     <row r="1" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="6" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="6" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="6" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B5" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="6" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B7" s="6" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B9" s="6" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="6" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B11" s="6" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B12" s="6" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B13" s="6" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B14" s="6" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B15" s="6" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B16" s="6" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B17" s="6" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B18" s="6" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B19" s="6" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B20" s="6" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B21" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B22" s="6" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B23" s="6" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B24" s="6" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B25" s="6" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B26" s="6" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B27" s="6" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="6" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="6" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B30" s="6" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B31" s="6" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B32" s="6" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B33" s="6" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B34" s="6" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B35" s="6" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B36" s="6" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B37" s="6" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B38" s="6" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B39" s="6" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B40" s="6" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B41" s="6" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B42" s="6" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B43" s="6" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B44" s="6" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B45" s="6" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B46" s="6" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B47" s="6" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B48" s="6" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B49" s="6" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B50" s="6" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B51" s="6" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B52" s="6" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B53" s="6" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B54" s="6" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B55" s="6" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B56" s="6" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B57" s="6" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B58" s="6" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B59" s="6" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B60" s="6" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B61" s="6" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -3720,7 +3521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BE7F4B-395F-49C6-BD46-AAA8F6C2F539}">
   <dimension ref="B1:C249"/>
   <sheetViews>
@@ -3736,586 +3537,586 @@
     <row r="1" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="6" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="6" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B4" s="6" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B5" s="6" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="6" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B7" s="6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B9" s="6" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="6" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B11" s="6" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B12" s="6" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B13" s="6" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B14" s="6" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B15" s="6" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B16" s="6" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B17" s="6" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B18" s="6" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B19" s="6" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B20" s="6" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B21" s="6" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B22" s="6" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B23" s="6" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B24" s="6" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B25" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B26" s="6" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B27" s="6" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="6" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="6" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B30" s="6" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B31" s="6" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B32" s="6" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B33" s="6" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B34" s="6" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B35" s="6" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B36" s="6" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B37" s="6" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B38" s="6" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B39" s="6" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B40" s="6" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B41" s="6" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B42" s="6" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B43" s="6" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B44" s="6" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B45" s="6" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B46" s="6" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B47" s="6" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B48" s="6" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B49" s="6" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B50" s="6" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B51" s="6" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B52" s="6" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B53" s="6" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B54" s="6" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B55" s="6" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B56" s="6" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B57" s="6" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B58" s="6" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B59" s="6" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B60" s="6" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B61" s="6" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B62" s="6" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B63" s="6" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
     </row>
     <row r="64" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B64" s="6" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B65" s="6" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B66" s="6" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B67" s="6" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B68" s="6" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B69" s="6" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B70" s="6" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B71" s="6" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B72" s="6" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B73" s="6" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B74" s="6" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -4498,7 +4299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7227DA8B-7030-4D60-A5B0-C4BC76065FC5}">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -4513,16 +4314,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="E1" s="5">
         <v>1</v>
@@ -4536,16 +4337,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="B2" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -4563,16 +4364,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -4586,16 +4387,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5">
@@ -4609,16 +4410,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5">
@@ -4632,50 +4433,50 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="B7" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="B8" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>